<commit_message>
- amend JSONModel::JSONModel(:resource) (where used) to include FA language & script, materials language & script - amend each sample csv / xlsx to add 4 new columns for FA language & script, materials language & script
</commit_message>
<xml_diff>
--- a/samples/Arrearage Template.xlsx
+++ b/samples/Arrearage Template.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelsmith/IdeaProjects/nla_staff_spreadsheet_importer/samples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD4EAE39-DBE2-BC4B-BD96-9581C1D871B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51120" windowHeight="24420"/>
+    <workbookView xWindow="42460" yWindow="5140" windowWidth="52140" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="127">
   <si>
     <t>series_statement</t>
   </si>
@@ -379,19 +385,45 @@
   <si>
     <t>Change to column mapping; change to column heading - now called 'Bib Id Collection level only'</t>
   </si>
+  <si>
+    <t>lang_materials</t>
+  </si>
+  <si>
+    <t>script_materials</t>
+  </si>
+  <si>
+    <t>finding_aid_language</t>
+  </si>
+  <si>
+    <t>finding_aid_script</t>
+  </si>
+  <si>
+    <t>Materials Language</t>
+  </si>
+  <si>
+    <t>Materials Script</t>
+  </si>
+  <si>
+    <t>Finding Aid Language</t>
+  </si>
+  <si>
+    <t>Finding Aid Script</t>
+  </si>
+  <si>
+    <t>Add - new column for mandatory Resource fields</t>
+  </si>
+  <si>
+    <t>Add - new column for mandatory Resource fields https://archivesspace-pilot.nla.gov.au/enumerations?id=26</t>
+  </si>
+  <si>
+    <t>Add - new column for mandatory Resource fields https://archivesspace-pilot.nla.gov.au/enumerations?id=74</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -430,6 +462,7 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -580,99 +613,99 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="31">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -748,6 +781,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1070,374 +1111,419 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:AMK15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AI1" sqref="AI1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="22.5" style="5" customWidth="1"/>
+    <col min="2" max="5" width="10.83203125" style="5"/>
+    <col min="6" max="6" width="17.1640625" style="5" customWidth="1"/>
+    <col min="7" max="11" width="10.83203125" style="5"/>
+    <col min="12" max="12" width="21.83203125" style="5" customWidth="1"/>
+    <col min="13" max="23" width="10.83203125" style="5"/>
+    <col min="24" max="24" width="17.33203125" style="5" customWidth="1"/>
+    <col min="25" max="1025" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="12" customFormat="1" ht="322">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:36" s="10" customFormat="1" ht="316" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9" t="s">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9" t="s">
+      <c r="M1" s="7"/>
+      <c r="N1" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9" t="s">
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9" t="s">
+      <c r="R1" s="7"/>
+      <c r="S1" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9" t="s">
+      <c r="T1" s="7"/>
+      <c r="U1" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Y1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="Z1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AA1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AB1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AC1" s="10" t="s">
+      <c r="AC1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AE1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AF1" s="7" t="s">
         <v>44</v>
       </c>
+      <c r="AG1" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="AJ1" s="9" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="2" spans="1:34" ht="38.25" customHeight="1">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:36" ht="38.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="14" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14" t="s">
+      <c r="M2" s="12"/>
+      <c r="N2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="Q2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14" t="s">
+      <c r="R2" s="12"/>
+      <c r="S2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14" t="s">
+      <c r="T2" s="12"/>
+      <c r="U2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="V2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="14" t="s">
+      <c r="W2" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="X2" s="17" t="s">
+      <c r="X2" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="Y2" s="17" t="s">
+      <c r="Y2" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="Z2" s="17" t="s">
+      <c r="Z2" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="AA2" s="17" t="s">
+      <c r="AA2" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="AB2" s="17" t="s">
+      <c r="AB2" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="AC2" s="17" t="s">
+      <c r="AC2" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="AD2" s="14" t="s">
+      <c r="AD2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="AE2" s="14" t="s">
+      <c r="AE2" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="AF2" s="18" t="s">
+      <c r="AF2" s="12" t="s">
         <v>51</v>
       </c>
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="16"/>
     </row>
-    <row r="3" spans="1:34" ht="90" customHeight="1">
-      <c r="A3" s="19" t="s">
+    <row r="3" spans="1:36" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="23" t="s">
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23" t="s">
+      <c r="M3" s="21"/>
+      <c r="N3" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="O3" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20" t="s">
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20" t="s">
+      <c r="R3" s="18"/>
+      <c r="S3" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20" t="s">
+      <c r="T3" s="18"/>
+      <c r="U3" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="V3" s="20" t="s">
+      <c r="V3" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="W3" s="20" t="s">
+      <c r="W3" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="X3" s="23" t="s">
+      <c r="X3" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="Y3" s="23" t="s">
+      <c r="Y3" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="Z3" s="23" t="s">
+      <c r="Z3" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="AA3" s="23" t="s">
+      <c r="AA3" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="AB3" s="23" t="s">
+      <c r="AB3" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="AC3" s="23" t="s">
+      <c r="AC3" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="AD3" s="20" t="s">
+      <c r="AD3" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="AE3" s="23" t="s">
+      <c r="AE3" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AF3" s="24" t="s">
+      <c r="AF3" s="21" t="s">
         <v>74</v>
       </c>
+      <c r="AG3" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH3" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI3" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="AJ3" s="22" t="s">
+        <v>123</v>
+      </c>
     </row>
-    <row r="4" spans="1:34" s="29" customFormat="1" ht="41.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:36" s="27" customFormat="1" ht="41.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="L4" s="26" t="s">
+      <c r="L4" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="M4" s="26" t="s">
+      <c r="M4" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="N4" s="26" t="s">
+      <c r="N4" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="O4" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="P4" s="26" t="s">
+      <c r="P4" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="26" t="s">
+      <c r="Q4" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="R4" s="26" t="s">
+      <c r="R4" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="S4" s="26" t="s">
+      <c r="S4" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="T4" s="26" t="s">
+      <c r="T4" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="U4" s="26" t="s">
+      <c r="U4" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="V4" s="26" t="s">
+      <c r="V4" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="W4" s="26" t="s">
+      <c r="W4" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="X4" s="26" t="s">
+      <c r="X4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="Y4" s="26" t="s">
+      <c r="Y4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="Z4" s="26" t="s">
+      <c r="Z4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="AA4" s="26" t="s">
+      <c r="AA4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="AB4" s="26" t="s">
+      <c r="AB4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="AC4" s="26" t="s">
+      <c r="AC4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AD4" s="26" t="s">
+      <c r="AD4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="AE4" s="26" t="s">
+      <c r="AE4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="AF4" s="26" t="s">
+      <c r="AF4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="AG4" s="26"/>
-      <c r="AH4" s="26"/>
+      <c r="AG4" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH4" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI4" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ4" s="24" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="5" spans="1:34" ht="57.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="30"/>
+    <row r="5" spans="1:36" ht="57.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1528,22 +1614,24 @@
       <c r="AE5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AF5" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="AG5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH5" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
-    <row r="6" spans="1:34" ht="15" thickTop="1"/>
-    <row r="7" spans="1:34" ht="14"/>
-    <row r="8" spans="1:34" ht="14"/>
-    <row r="9" spans="1:34" ht="14"/>
-    <row r="10" spans="1:34" ht="14"/>
-    <row r="11" spans="1:34" ht="14"/>
-    <row r="12" spans="1:34" ht="14"/>
-    <row r="13" spans="1:34" ht="14"/>
-    <row r="14" spans="1:34" ht="14"/>
-    <row r="15" spans="1:34" ht="14"/>
+    <row r="6" spans="1:36" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="G3:J3"/>

</xml_diff>